<commit_message>
Add PRE Ultra Rares
</commit_message>
<xml_diff>
--- a/docs/PocketCards.xlsx
+++ b/docs/PocketCards.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34162F37-3D6C-4669-8788-E752D7127257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE02A4A-51AC-49E2-8F8D-4AC4FD337A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E655B03A-0615-48A1-906C-9E73CC102A05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E655B03A-0615-48A1-906C-9E73CC102A05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Genetic Apex" sheetId="9" r:id="rId1"/>
-    <sheet name="Promo-A" sheetId="12" r:id="rId2"/>
-    <sheet name="Helper" sheetId="11" r:id="rId3"/>
+    <sheet name="A1" sheetId="9" r:id="rId1"/>
+    <sheet name="A1a" sheetId="13" r:id="rId2"/>
+    <sheet name="Promo-A" sheetId="12" r:id="rId3"/>
+    <sheet name="Helper" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="135">
   <si>
     <t>Grass</t>
   </si>
@@ -298,9 +299,6 @@
     <t>Special_Art_ex</t>
   </si>
   <si>
-    <t>Immersive_Art_ex</t>
-  </si>
-  <si>
     <t>Gold_ex</t>
   </si>
   <si>
@@ -374,6 +372,78 @@
   </si>
   <si>
     <t>Holo</t>
+  </si>
+  <si>
+    <t>Chansey</t>
+  </si>
+  <si>
+    <t>Lapras ex</t>
+  </si>
+  <si>
+    <t>Magnemite</t>
+  </si>
+  <si>
+    <t>Volcarona</t>
+  </si>
+  <si>
+    <t>TCG Pocket Rarity Diamond.png</t>
+  </si>
+  <si>
+    <t>TCG Pocket Rarity Diamond.pngTCG Pocket Rarity Diamond.png</t>
+  </si>
+  <si>
+    <t>Serperior</t>
+  </si>
+  <si>
+    <t>TCG Pocket Rarity Diamond.pngTCG Pocket Rarity Diamond.pngTCG Pocket Rarity Diamond.png</t>
+  </si>
+  <si>
+    <t>Salandit</t>
+  </si>
+  <si>
+    <t>Dedenne</t>
+  </si>
+  <si>
+    <t>Aerodactylex</t>
+  </si>
+  <si>
+    <t>Marshadow</t>
+  </si>
+  <si>
+    <t>Tauros</t>
+  </si>
+  <si>
+    <t>Budding Expeditioner</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>Celebi ex</t>
+  </si>
+  <si>
+    <t>Gyarados ex</t>
+  </si>
+  <si>
+    <t>Mew ex</t>
+  </si>
+  <si>
+    <t>Aerodactyl ex</t>
+  </si>
+  <si>
+    <t>Pidgeot ex</t>
+  </si>
+  <si>
+    <t>Celebi</t>
+  </si>
+  <si>
+    <t>Mythical_Island</t>
+  </si>
+  <si>
+    <t>Immersive_Art</t>
   </si>
 </sst>
 </file>
@@ -409,9 +479,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -728,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F418748F-D738-402F-B110-C874A568DB73}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,11 +2452,11 @@
         <v>48</v>
       </c>
       <c r="F69" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>new PocketCard("Charizard ex", Pokedex.Charizard, PocketRarity.Immersive_Art_ex, Types.Fire, Sets.Genetic_Apex, 280),</v>
+        <v>new PocketCard("Charizard ex", Pokedex.Charizard, PocketRarity.Immersive_Art, Types.Fire, Sets.Genetic_Apex, 280),</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2407,11 +2476,11 @@
         <v>48</v>
       </c>
       <c r="F70" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>new PocketCard("Pikachu ex", Pokedex.Pikachu, PocketRarity.Immersive_Art_ex, Types.Lightning, Sets.Genetic_Apex, 281),</v>
+        <v>new PocketCard("Pikachu ex", Pokedex.Pikachu, PocketRarity.Immersive_Art, Types.Lightning, Sets.Genetic_Apex, 281),</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2431,11 +2500,11 @@
         <v>48</v>
       </c>
       <c r="F71" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>new PocketCard("Mewtwo ex", Pokedex.Mewtwo, PocketRarity.Immersive_Art_ex, Types.Psychic, Sets.Genetic_Apex, 282),</v>
+        <v>new PocketCard("Mewtwo ex", Pokedex.Mewtwo, PocketRarity.Immersive_Art, Types.Psychic, Sets.Genetic_Apex, 282),</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2455,7 +2524,7 @@
         <v>48</v>
       </c>
       <c r="F72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
@@ -2479,7 +2548,7 @@
         <v>48</v>
       </c>
       <c r="F73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
@@ -2503,7 +2572,7 @@
         <v>48</v>
       </c>
       <c r="F74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
@@ -2527,15 +2596,15 @@
         <v>48</v>
       </c>
       <c r="F75" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v>new PocketCard("Mew", Pokedex.Mew, PocketRarity.Immersive_Art_ex, Types.Psychic, Sets.Genetic_Apex, 283),</v>
+        <v>new PocketCard("Mew", Pokedex.Mew, PocketRarity.Immersive_Art, Types.Psychic, Sets.Genetic_Apex, 283),</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+      <c r="A76">
         <v>3</v>
       </c>
       <c r="B76" t="s">
@@ -2551,7 +2620,7 @@
         <v>48</v>
       </c>
       <c r="F76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
@@ -2559,14 +2628,14 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+      <c r="A77">
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D77" t="s">
         <v>0</v>
@@ -2575,7 +2644,7 @@
         <v>48</v>
       </c>
       <c r="F77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
@@ -2583,14 +2652,14 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+      <c r="A78">
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D78" t="s">
         <v>0</v>
@@ -2599,7 +2668,7 @@
         <v>48</v>
       </c>
       <c r="F78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
@@ -2607,14 +2676,14 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+      <c r="A79">
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
         <v>0</v>
@@ -2623,7 +2692,7 @@
         <v>48</v>
       </c>
       <c r="F79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
@@ -2631,14 +2700,14 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+      <c r="A80">
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D80" t="s">
         <v>0</v>
@@ -2647,7 +2716,7 @@
         <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
@@ -2655,7 +2724,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
+      <c r="A81">
         <v>22</v>
       </c>
       <c r="B81" t="s">
@@ -2671,7 +2740,7 @@
         <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
@@ -2679,7 +2748,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
+      <c r="A82">
         <v>35</v>
       </c>
       <c r="B82" t="s">
@@ -2695,7 +2764,7 @@
         <v>48</v>
       </c>
       <c r="F82" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
@@ -2703,7 +2772,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
+      <c r="A83">
         <v>40</v>
       </c>
       <c r="B83" t="s">
@@ -2719,7 +2788,7 @@
         <v>48</v>
       </c>
       <c r="F83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
@@ -2727,14 +2796,14 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
+      <c r="A84">
         <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
@@ -2743,7 +2812,7 @@
         <v>48</v>
       </c>
       <c r="F84" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
@@ -2751,7 +2820,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
+      <c r="A85">
         <v>46</v>
       </c>
       <c r="B85" t="s">
@@ -2767,7 +2836,7 @@
         <v>48</v>
       </c>
       <c r="F85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
@@ -2775,7 +2844,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
+      <c r="A86">
         <v>55</v>
       </c>
       <c r="B86" t="s">
@@ -2791,7 +2860,7 @@
         <v>48</v>
       </c>
       <c r="F86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
@@ -2799,14 +2868,14 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
+      <c r="A87">
         <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
@@ -2815,7 +2884,7 @@
         <v>48</v>
       </c>
       <c r="F87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
@@ -2823,7 +2892,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
+      <c r="A88">
         <v>78</v>
       </c>
       <c r="B88" t="s">
@@ -2839,7 +2908,7 @@
         <v>48</v>
       </c>
       <c r="F88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
@@ -2847,7 +2916,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
+      <c r="A89">
         <v>79</v>
       </c>
       <c r="B89" t="s">
@@ -2863,7 +2932,7 @@
         <v>48</v>
       </c>
       <c r="F89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
@@ -2871,14 +2940,14 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
+      <c r="A90">
         <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
@@ -2887,7 +2956,7 @@
         <v>48</v>
       </c>
       <c r="F90" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
@@ -2895,14 +2964,14 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
+      <c r="A91">
         <v>82</v>
       </c>
       <c r="B91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
@@ -2911,7 +2980,7 @@
         <v>48</v>
       </c>
       <c r="F91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
@@ -2919,7 +2988,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
+      <c r="A92">
         <v>83</v>
       </c>
       <c r="B92" t="s">
@@ -2935,7 +3004,7 @@
         <v>48</v>
       </c>
       <c r="F92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
@@ -2943,14 +3012,14 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
+      <c r="A93">
         <v>89</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
@@ -2959,7 +3028,7 @@
         <v>48</v>
       </c>
       <c r="F93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
@@ -2967,14 +3036,14 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
+      <c r="A94">
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D94" t="s">
         <v>8</v>
@@ -2983,7 +3052,7 @@
         <v>48</v>
       </c>
       <c r="F94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
@@ -2991,14 +3060,14 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
+      <c r="A95">
         <v>98</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
@@ -3007,7 +3076,7 @@
         <v>48</v>
       </c>
       <c r="F95" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
@@ -3015,14 +3084,14 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
+      <c r="A96">
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D96" t="s">
         <v>8</v>
@@ -3031,7 +3100,7 @@
         <v>48</v>
       </c>
       <c r="F96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
@@ -3039,7 +3108,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
+      <c r="A97">
         <v>103</v>
       </c>
       <c r="B97" t="s">
@@ -3055,7 +3124,7 @@
         <v>48</v>
       </c>
       <c r="F97" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
@@ -3063,14 +3132,14 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
+      <c r="A98">
         <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
@@ -3079,7 +3148,7 @@
         <v>48</v>
       </c>
       <c r="F98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="1"/>
@@ -3087,7 +3156,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
+      <c r="A99">
         <v>117</v>
       </c>
       <c r="B99" t="s">
@@ -3103,7 +3172,7 @@
         <v>48</v>
       </c>
       <c r="F99" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="1"/>
@@ -3111,7 +3180,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
+      <c r="A100">
         <v>122</v>
       </c>
       <c r="B100" t="s">
@@ -3127,7 +3196,7 @@
         <v>48</v>
       </c>
       <c r="F100" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="1"/>
@@ -3135,14 +3204,14 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
+      <c r="A101">
         <v>125</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -3151,7 +3220,7 @@
         <v>48</v>
       </c>
       <c r="F101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="1"/>
@@ -3159,7 +3228,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
+      <c r="A102">
         <v>128</v>
       </c>
       <c r="B102" t="s">
@@ -3175,7 +3244,7 @@
         <v>48</v>
       </c>
       <c r="F102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="1"/>
@@ -3183,14 +3252,14 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
+      <c r="A103">
         <v>132</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D103" t="s">
         <v>9</v>
@@ -3199,7 +3268,7 @@
         <v>48</v>
       </c>
       <c r="F103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
@@ -3207,7 +3276,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
+      <c r="A104">
         <v>145</v>
       </c>
       <c r="B104" t="s">
@@ -3223,7 +3292,7 @@
         <v>48</v>
       </c>
       <c r="F104" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="1"/>
@@ -3231,14 +3300,14 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
+      <c r="A105">
         <v>149</v>
       </c>
       <c r="B105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -3247,7 +3316,7 @@
         <v>48</v>
       </c>
       <c r="F105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
@@ -3255,14 +3324,14 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="1">
+      <c r="A106">
         <v>159</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
@@ -3271,7 +3340,7 @@
         <v>48</v>
       </c>
       <c r="F106" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
@@ -3279,7 +3348,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
+      <c r="A107">
         <v>168</v>
       </c>
       <c r="B107" t="s">
@@ -3295,7 +3364,7 @@
         <v>48</v>
       </c>
       <c r="F107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="1"/>
@@ -3303,7 +3372,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="1">
+      <c r="A108">
         <v>171</v>
       </c>
       <c r="B108" t="s">
@@ -3319,7 +3388,7 @@
         <v>48</v>
       </c>
       <c r="F108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="1"/>
@@ -3327,14 +3396,14 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
+      <c r="A109">
         <v>175</v>
       </c>
       <c r="B109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D109" t="s">
         <v>11</v>
@@ -3343,7 +3412,7 @@
         <v>48</v>
       </c>
       <c r="F109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="1"/>
@@ -3351,7 +3420,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="1">
+      <c r="A110">
         <v>177</v>
       </c>
       <c r="B110" t="s">
@@ -3367,7 +3436,7 @@
         <v>48</v>
       </c>
       <c r="F110" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="1"/>
@@ -3375,23 +3444,23 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
+      <c r="A111">
         <v>182</v>
       </c>
       <c r="B111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E111" t="s">
         <v>48</v>
       </c>
       <c r="F111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="1"/>
@@ -3399,7 +3468,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
+      <c r="A112">
         <v>185</v>
       </c>
       <c r="B112" t="s">
@@ -3415,7 +3484,7 @@
         <v>48</v>
       </c>
       <c r="F112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="1"/>
@@ -3423,7 +3492,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
+      <c r="A113">
         <v>188</v>
       </c>
       <c r="B113" t="s">
@@ -3439,7 +3508,7 @@
         <v>48</v>
       </c>
       <c r="F113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="1"/>
@@ -3447,14 +3516,14 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
+      <c r="A114">
         <v>203</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D114" t="s">
         <v>13</v>
@@ -3463,7 +3532,7 @@
         <v>48</v>
       </c>
       <c r="F114" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="1"/>
@@ -3471,7 +3540,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
+      <c r="A115">
         <v>205</v>
       </c>
       <c r="B115" t="s">
@@ -3487,7 +3556,7 @@
         <v>48</v>
       </c>
       <c r="F115" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="1"/>
@@ -3495,14 +3564,14 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
+      <c r="A116">
         <v>210</v>
       </c>
       <c r="B116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D116" t="s">
         <v>13</v>
@@ -3511,7 +3580,7 @@
         <v>48</v>
       </c>
       <c r="F116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="1"/>
@@ -3519,7 +3588,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
+      <c r="A117">
         <v>211</v>
       </c>
       <c r="B117" t="s">
@@ -3535,7 +3604,7 @@
         <v>48</v>
       </c>
       <c r="F117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="1"/>
@@ -3548,11 +3617,791 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454B3CC1-CBE7-4E42-AAB5-34F162C839A5}">
+  <dimension ref="A1:T31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="str">
+        <f>"new PocketCard(""" &amp; B1 &amp; """, Pokedex." &amp; C1 &amp; ", PocketRarity." &amp; F1 &amp; ", Types." &amp; D1 &amp; ", Sets." &amp; E1 &amp; ", " &amp; A1 &amp; "),"</f>
+        <v>new PocketCard("Celebi ex", Pokedex.Celebi, PocketRarity.ex, Types.Grass, Sets.Mythical_Island, 3),</v>
+      </c>
+      <c r="S1" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" t="str">
+        <f>IF(OR(S1 = "TCG Pocket Rarity Diamond.png", S1 = "TCG Pocket Rarity Diamond.pngTCG Pocket Rarity Diamond.png"), "", "&lt;- DEZE")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G31" si="0">"new PocketCard(""" &amp; B2 &amp; """, Pokedex." &amp; C2 &amp; ", PocketRarity." &amp; F2 &amp; ", Types." &amp; D2 &amp; ", Sets." &amp; E2 &amp; ", " &amp; A2 &amp; "),"</f>
+        <v>new PocketCard("Serperior", Pokedex.Serperior, PocketRarity.Holo, Types.Grass, Sets.Mythical_Island, 6),</v>
+      </c>
+      <c r="S2" t="s">
+        <v>116</v>
+      </c>
+      <c r="T2" t="str">
+        <f t="shared" ref="T2:T3" si="1">IF(OR(S2 = "TCG Pocket Rarity Diamond.png", S2 = "TCG Pocket Rarity Diamond.pngTCG Pocket Rarity Diamond.png"), "", "&lt;- DEZE")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Volcarona", Pokedex.Volcarona, PocketRarity.Holo, Types.Fire, Sets.Mythical_Island, 14),</v>
+      </c>
+      <c r="S3" t="s">
+        <v>118</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;- DEZE</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Gyarados ex", Pokedex.Gyarados, PocketRarity.ex, Types.Water, Sets.Mythical_Island, 18),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Vaporeon", Pokedex.Vaporeon, PocketRarity.Holo, Types.Water, Sets.Mythical_Island, 19),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Raichu", Pokedex.Raichu, PocketRarity.Holo, Types.Lightning, Sets.Mythical_Island, 26),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Mew", Pokedex.Mew, PocketRarity.Holo, Types.Psychic, Sets.Mythical_Island, 31),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Mew ex", Pokedex.Mew, PocketRarity.ex, Types.Psychic, Sets.Mythical_Island, 32),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Golem", Pokedex.Golem, PocketRarity.Holo, Types.Fighting, Sets.Mythical_Island, 45),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Aerodactyl ex", Pokedex.Aerodactyl, PocketRarity.ex, Types.Fighting, Sets.Mythical_Island, 46),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Marshadow", Pokedex.Marshadow, PocketRarity.Holo, Types.Fighting, Sets.Mythical_Island, 47),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Pidgeot ex", Pokedex.Pidgeot, PocketRarity.ex, Types.Colorless, Sets.Mythical_Island, 59),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Tauros", Pokedex.Tauros, PocketRarity.Holo, Types.Colorless, Sets.Mythical_Island, 60),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Exeggutor", Pokedex.Exeggutor, PocketRarity.Special_Art_Pokémon, Types.Grass, Sets.Mythical_Island, 69),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Serperior", Pokedex.Serperior, PocketRarity.Special_Art_Pokémon, Types.Grass, Sets.Mythical_Island, 70),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Salandit", Pokedex.Salandit, PocketRarity.Special_Art_Pokémon, Types.Fire, Sets.Mythical_Island, 71),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Vaporeon", Pokedex.Vaporeon, PocketRarity.Special_Art_Pokémon, Types.Water, Sets.Mythical_Island, 72),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Dedenne", Pokedex.Dedenne, PocketRarity.Special_Art_Pokémon, Types.Lightning, Sets.Mythical_Island, 73),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Marshadow", Pokedex.Marshadow, PocketRarity.Special_Art_Pokémon, Types.Fighting, Sets.Mythical_Island, 74),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Celebi ex", Pokedex.Celebi, PocketRarity.Full_Art_ex, Types.Grass, Sets.Mythical_Island, 75),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Gyarados ex", Pokedex.Gyarados, PocketRarity.Full_Art_ex, Types.Water, Sets.Mythical_Island, 76),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Mew ex", Pokedex.Mew, PocketRarity.Full_Art_ex, Types.Psychic, Sets.Mythical_Island, 77),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Aerodactyl ex", Pokedex.Aerodactyl, PocketRarity.Full_Art_ex, Types.Fighting, Sets.Mythical_Island, 78),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Pidgeot ex", Pokedex.Pidgeot, PocketRarity.Full_Art_ex, Types.Colorless, Sets.Mythical_Island, 79),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Budding Expeditioner", Pokedex.NVT, PocketRarity.Full_Art_Trainer, Types.Supporter, Sets.Mythical_Island, 80),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Blue", Pokedex.NVT, PocketRarity.Full_Art_Trainer, Types.Supporter, Sets.Mythical_Island, 81),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Leaf", Pokedex.NVT, PocketRarity.Full_Art_Trainer, Types.Supporter, Sets.Mythical_Island, 82),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Mew ex", Pokedex.Mew, PocketRarity.Special_Art_ex, Types.Psychic, Sets.Mythical_Island, 83),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Aerodactylex", Pokedex.Aerodactyl, PocketRarity.Special_Art_ex, Types.Fighting, Sets.Mythical_Island, 84),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Celebi ex", Pokedex.Celebi, PocketRarity.Immersive_Art, Types.Grass, Sets.Mythical_Island, 85),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Mew ex", Pokedex.Mew, PocketRarity.Gold_ex, Types.Psychic, Sets.Mythical_Island, 86),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B7D611-A3FA-4E15-87B8-0182AC9E2B2A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3571,13 +4420,13 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>65</v>
       </c>
       <c r="G1" t="str">
-        <f t="shared" ref="G1:G3" si="0">"new PocketCard(""" &amp; B1 &amp; """, Pokedex." &amp; C1 &amp; ", PocketRarity." &amp; F1 &amp; ", Types." &amp; D1 &amp; ", Sets." &amp; E1 &amp; ", " &amp; A1 &amp; "),"</f>
+        <f t="shared" ref="G1:G16" si="0">"new PocketCard(""" &amp; B1 &amp; """, Pokedex." &amp; C1 &amp; ", PocketRarity." &amp; F1 &amp; ", Types." &amp; D1 &amp; ", Sets." &amp; E1 &amp; ", " &amp; A1 &amp; "),"</f>
         <v>new PocketCard("Pikachu", Pokedex.Pikachu, PocketRarity.Special_Art_Pokémon, Types.Lightning, Sets.Promo_A, 9),</v>
       </c>
     </row>
@@ -3595,7 +4444,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
         <v>65</v>
@@ -3619,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -3627,6 +4476,318 @@
       <c r="G3" t="str">
         <f t="shared" si="0"/>
         <v>new PocketCard("Venusaur", Pokedex.Venusaur, PocketRarity.Special_Art_Pokémon, Types.Grass, Sets.Promo_A, 18),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Chansey", Pokedex.Chansey, PocketRarity.Holo, Types.Colorless, Sets.Promo_A, 11),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Meowth", Pokedex.Meowth, PocketRarity.Holo, Types.Colorless, Sets.Promo_A, 12),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Butterfree", Pokedex.Butterfree, PocketRarity.Holo, Types.Grass, Sets.Promo_A, 13),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Lapras ex", Pokedex.Lapras, PocketRarity.ex, Types.Water, Sets.Promo_A, 14),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Greninja", Pokedex.Greninja, PocketRarity.Holo, Types.Water, Sets.Promo_A, 19),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Bulbasaur", Pokedex.Bulbasaur, PocketRarity.Holo, Types.Grass, Sets.Promo_A, 23),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Magnemite", Pokedex.Magnemite, PocketRarity.Holo, Types.Lightning, Sets.Promo_A, 24),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Moltres ex", Pokedex.Moltres, PocketRarity.ex, Types.Fire, Sets.Promo_A, 25),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Pikachu", Pokedex.Pikachu, PocketRarity.Special_Art_Pokémon, Types.Lightning, Sets.Promo_A, 26),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Volcarona", Pokedex.Volcarona, PocketRarity.Holo, Types.Fire, Sets.Promo_A, 28),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Blastoise", Pokedex.Blastoise, PocketRarity.Special_Art_Pokémon, Types.Water, Sets.Promo_A, 29),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Charmander", Pokedex.Charmander, PocketRarity.Holo, Types.Fire, Sets.Promo_A, 32),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>new PocketCard("Squirtle", Pokedex.Squirtle, PocketRarity.Holo, Types.Water, Sets.Promo_A, 33),</v>
       </c>
     </row>
   </sheetData>
@@ -3634,7 +4795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5254EFC-8A47-4896-9112-37C6F31202C5}">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>